<commit_message>
move & look instruction added
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuari\Desktop\Arena_Game\ARENA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuari\Desktop\Arena_Game\ARENA\Arena_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>Objects/Creatures added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">map(10%) &amp; player added </t>
+  </si>
+  <si>
+    <t>game map &amp; quit instruction</t>
   </si>
 </sst>
 </file>
@@ -442,10 +448,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -453,154 +459,208 @@
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="D2" s="4"/>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="4"/>
+      <c r="F2" s="4"/>
+      <c r="G2" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="2"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="2">
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="2">
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="4"/>
-      <c r="E5" s="2">
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="2">
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D6" s="4"/>
-      <c r="E6" s="2">
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="2">
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D7" s="4"/>
-      <c r="E7" s="2">
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C8" s="4"/>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C8" s="5" t="s">
+        <v>8</v>
+      </c>
       <c r="D8" s="4"/>
-      <c r="E8" s="2"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C9" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C9" s="5" t="s">
+        <v>9</v>
+      </c>
       <c r="D9" s="4"/>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C10" s="4"/>
       <c r="D10" s="4"/>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="2"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C12" s="4"/>
       <c r="D12" s="4"/>
-      <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E12" s="4"/>
+      <c r="F12" s="4"/>
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C14" s="4"/>
       <c r="D14" s="4"/>
-      <c r="E14" s="2"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
       <c r="D16" s="4"/>
-      <c r="E16" s="2"/>
-    </row>
-    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E16" s="4"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="2"/>
-    </row>
-    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E17" s="4"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="2"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
       <c r="D18" s="4"/>
-      <c r="E18" s="2"/>
-    </row>
-    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="2"/>
+    </row>
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
       <c r="D19" s="4"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E19" s="4"/>
+      <c r="F19" s="4"/>
+      <c r="G19" s="2"/>
+    </row>
+    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="2"/>
-    </row>
-    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E20" s="4"/>
+      <c r="F20" s="4"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
-      <c r="E21" s="2"/>
-    </row>
-    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E21" s="4"/>
+      <c r="F21" s="4"/>
+      <c r="G21" s="2"/>
+    </row>
+    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
       <c r="D22" s="4"/>
-      <c r="E22" s="2"/>
-    </row>
-    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E22" s="4"/>
+      <c r="F22" s="4"/>
+      <c r="G22" s="2"/>
+    </row>
+    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="2"/>
-    </row>
-    <row r="24" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="E23" s="4"/>
+      <c r="F23" s="4"/>
+      <c r="G23" s="2"/>
+    </row>
+    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="2"/>
-    </row>
-    <row r="26" spans="3:5" x14ac:dyDescent="0.25">
-      <c r="D26" s="1" t="s">
+      <c r="E24" s="4"/>
+      <c r="F24" s="4"/>
+      <c r="G24" s="2"/>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E26" s="1">
-        <f>SUM(E4:E24)</f>
-        <v>2.35</v>
+      <c r="G26" s="1">
+        <f>SUM(G4:G24)</f>
+        <v>3.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pick & look & class update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -54,6 +54,21 @@
   </si>
   <si>
     <t>game map &amp; quit instruction</t>
+  </si>
+  <si>
+    <t>move &amp; look instruction added</t>
+  </si>
+  <si>
+    <t>pick instruction added</t>
+  </si>
+  <si>
+    <t>look update</t>
+  </si>
+  <si>
+    <t>object added to the game data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">general update (class TYPES) </t>
   </si>
 </sst>
 </file>
@@ -451,7 +466,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -550,39 +565,59 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C10" s="4"/>
+      <c r="C10" s="5" t="s">
+        <v>10</v>
+      </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="4"/>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C11" s="4"/>
+      <c r="C11" s="5" t="s">
+        <v>11</v>
+      </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
-      <c r="G11" s="2"/>
+      <c r="G11" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C12" s="4"/>
+      <c r="C12" s="5" t="s">
+        <v>12</v>
+      </c>
       <c r="D12" s="4"/>
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
-      <c r="G12" s="2"/>
+      <c r="G12" s="2">
+        <v>0.3</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C13" s="4"/>
+      <c r="C13" s="5" t="s">
+        <v>13</v>
+      </c>
       <c r="D13" s="4"/>
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
-      <c r="G13" s="2"/>
+      <c r="G13" s="2">
+        <v>0.4</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C14" s="4"/>
+      <c r="C14" s="5" t="s">
+        <v>14</v>
+      </c>
       <c r="D14" s="4"/>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>
-      <c r="G14" s="2"/>
+      <c r="G14" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C15" s="4"/>
@@ -660,7 +695,7 @@
       </c>
       <c r="G26" s="1">
         <f>SUM(G4:G24)</f>
-        <v>3.65</v>
+        <v>9.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pull added & pick repaired
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t xml:space="preserve">general update (class TYPES) </t>
+  </si>
+  <si>
+    <t>Goblin added and creature functions update</t>
   </si>
 </sst>
 </file>
@@ -465,8 +468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -620,11 +623,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C15" s="4"/>
+      <c r="C15" s="5" t="s">
+        <v>15</v>
+      </c>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
@@ -695,10 +702,11 @@
       </c>
       <c r="G26" s="1">
         <f>SUM(G4:G24)</f>
-        <v>9.15</v>
+        <v>11.15</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
npc deleted & merchant & talk instruction added
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -72,6 +72,12 @@
   </si>
   <si>
     <t>Goblin added and creature functions update</t>
+  </si>
+  <si>
+    <t>pull added &amp; pick repaired</t>
+  </si>
+  <si>
+    <t>npc deleted &amp; merchant &amp; talk instruction added</t>
   </si>
 </sst>
 </file>
@@ -469,7 +475,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,18 +640,26 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="C16" s="4"/>
+      <c r="C16" s="5" t="s">
+        <v>16</v>
+      </c>
       <c r="D16" s="4"/>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="4"/>
+      <c r="C17" s="5" t="s">
+        <v>17</v>
+      </c>
       <c r="D17" s="4"/>
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
-      <c r="G17" s="2"/>
+      <c r="G17" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="4"/>
@@ -702,7 +716,7 @@
       </c>
       <c r="G26" s="1">
         <f>SUM(G4:G24)</f>
-        <v>11.15</v>
+        <v>13.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
equip intruction partially added
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -78,6 +78,9 @@
   </si>
   <si>
     <t>npc deleted &amp; merchant &amp; talk instruction added</t>
+  </si>
+  <si>
+    <t>equip instruction &amp; functionality added</t>
   </si>
 </sst>
 </file>
@@ -475,7 +478,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,11 +665,15 @@
       </c>
     </row>
     <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C18" s="4"/>
+      <c r="C18" s="5" t="s">
+        <v>18</v>
+      </c>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
       <c r="F18" s="4"/>
-      <c r="G18" s="2"/>
+      <c r="G18" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="4"/>
@@ -716,7 +723,7 @@
       </c>
       <c r="G26" s="1">
         <f>SUM(G4:G24)</f>
-        <v>13.65</v>
+        <v>15.65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pull & pick instructions repaired
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>unequip instruction added</t>
+  </si>
+  <si>
+    <t>pull &amp; pick instructions repaired</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -704,11 +707,15 @@
       </c>
     </row>
     <row r="21" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C21" s="4"/>
+      <c r="C21" s="5" t="s">
+        <v>21</v>
+      </c>
       <c r="D21" s="4"/>
       <c r="E21" s="4"/>
       <c r="F21" s="4"/>
-      <c r="G21" s="2"/>
+      <c r="G21" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C22" s="4"/>
@@ -737,7 +744,7 @@
       </c>
       <c r="G26" s="1">
         <f>SUM(G4:G24)</f>
-        <v>18.600000000000001</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
talk virtual function instruction repaired
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>pull &amp; pick instructions repaired</t>
+  </si>
+  <si>
+    <t>talk virtual function instruction repaired</t>
   </si>
 </sst>
 </file>
@@ -487,7 +490,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -718,11 +721,15 @@
       </c>
     </row>
     <row r="22" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C22" s="4"/>
+      <c r="C22" s="5" t="s">
+        <v>22</v>
+      </c>
       <c r="D22" s="4"/>
       <c r="E22" s="4"/>
       <c r="F22" s="4"/>
-      <c r="G22" s="2"/>
+      <c r="G22" s="2">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C23" s="4"/>
@@ -744,7 +751,7 @@
       </c>
       <c r="G26" s="1">
         <f>SUM(G4:G24)</f>
-        <v>19.100000000000001</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
user look_it & sell/buy update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -93,6 +93,12 @@
   </si>
   <si>
     <t>talk virtual function instruction repaired</t>
+  </si>
+  <si>
+    <t>merchant talk action update (40%)</t>
+  </si>
+  <si>
+    <t>user look_it &amp; sell/buy update</t>
   </si>
 </sst>
 </file>
@@ -487,10 +493,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,26 +738,34 @@
       </c>
     </row>
     <row r="23" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C23" s="4"/>
+      <c r="C23" s="5" t="s">
+        <v>23</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
       <c r="F23" s="4"/>
-      <c r="G23" s="2"/>
+      <c r="G23" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="24" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C24" s="4"/>
+      <c r="C24" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="D24" s="4"/>
       <c r="E24" s="4"/>
       <c r="F24" s="4"/>
-      <c r="G24" s="2"/>
-    </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F26" s="1" t="s">
+      <c r="G24" s="2">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F29" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G26" s="1">
+      <c r="G29" s="1">
         <f>SUM(G4:G24)</f>
-        <v>19.600000000000001</v>
+        <v>21.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
directional look & levels system added
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>user look_it &amp; sell/buy update</t>
+  </si>
+  <si>
+    <t>directional look &amp; levles system added</t>
   </si>
 </sst>
 </file>
@@ -495,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -759,13 +762,45 @@
         <v>0.7</v>
       </c>
     </row>
+    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C25" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="4"/>
+      <c r="G25" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="4"/>
+      <c r="G26" s="2"/>
+    </row>
+    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C27" s="5"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="4"/>
+      <c r="G27" s="2"/>
+    </row>
+    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C28" s="5"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="4"/>
+      <c r="G28" s="2"/>
+    </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
       <c r="F29" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G29" s="1">
-        <f>SUM(G4:G24)</f>
-        <v>21.8</v>
+        <f>SUM(G4:G25)</f>
+        <v>22.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
creatures states update & Crafter NPC base code added
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t>directional look &amp; levles system added</t>
+  </si>
+  <si>
+    <t>game output system &amp; levels update</t>
+  </si>
+  <si>
+    <t>creatures states update &amp; Crafter NPC base code</t>
   </si>
 </sst>
 </file>
@@ -496,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -774,18 +780,26 @@
       </c>
     </row>
     <row r="26" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C26" s="5"/>
+      <c r="C26" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="D26" s="4"/>
       <c r="E26" s="4"/>
       <c r="F26" s="4"/>
-      <c r="G26" s="2"/>
+      <c r="G26" s="2">
+        <v>1.2</v>
+      </c>
     </row>
     <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" s="5"/>
+      <c r="C27" s="5" t="s">
+        <v>27</v>
+      </c>
       <c r="D27" s="4"/>
       <c r="E27" s="4"/>
       <c r="F27" s="4"/>
-      <c r="G27" s="2"/>
+      <c r="G27" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C28" s="5"/>
@@ -795,12 +809,75 @@
       <c r="G28" s="2"/>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F29" s="1" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="2"/>
+    </row>
+    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C30" s="5"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4"/>
+      <c r="G30" s="2"/>
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="5"/>
+      <c r="D31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="4"/>
+      <c r="G31" s="2"/>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="5"/>
+      <c r="D32" s="4"/>
+      <c r="E32" s="4"/>
+      <c r="F32" s="4"/>
+      <c r="G32" s="2"/>
+    </row>
+    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C33" s="5"/>
+      <c r="D33" s="4"/>
+      <c r="E33" s="4"/>
+      <c r="F33" s="4"/>
+      <c r="G33" s="2"/>
+    </row>
+    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C34" s="5"/>
+      <c r="D34" s="4"/>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="2"/>
+    </row>
+    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C35" s="5"/>
+      <c r="D35" s="4"/>
+      <c r="E35" s="4"/>
+      <c r="F35" s="4"/>
+      <c r="G35" s="2"/>
+    </row>
+    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C36" s="5"/>
+      <c r="D36" s="4"/>
+      <c r="E36" s="4"/>
+      <c r="F36" s="4"/>
+      <c r="G36" s="2"/>
+    </row>
+    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C37" s="5"/>
+      <c r="D37" s="4"/>
+      <c r="E37" s="4"/>
+      <c r="F37" s="4"/>
+      <c r="G37" s="2"/>
+    </row>
+    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="F39" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G29" s="1">
-        <f>SUM(G4:G25)</f>
-        <v>22.8</v>
+      <c r="G39" s="1">
+        <f>SUM(G4:G27)</f>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Runner update (80%) & general data update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -108,6 +108,12 @@
   </si>
   <si>
     <t>creatures states update &amp; Crafter NPC base code</t>
+  </si>
+  <si>
+    <t>base Runner &amp; general update</t>
+  </si>
+  <si>
+    <t>Runner update(80%) &amp; general data update</t>
   </si>
 </sst>
 </file>
@@ -505,7 +511,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -802,18 +808,26 @@
       </c>
     </row>
     <row r="28" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C28" s="5"/>
+      <c r="C28" s="5" t="s">
+        <v>28</v>
+      </c>
       <c r="D28" s="4"/>
       <c r="E28" s="4"/>
       <c r="F28" s="4"/>
-      <c r="G28" s="2"/>
+      <c r="G28" s="2">
+        <v>2.2000000000000002</v>
+      </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" s="5"/>
+      <c r="C29" s="5" t="s">
+        <v>29</v>
+      </c>
       <c r="D29" s="4"/>
       <c r="E29" s="4"/>
       <c r="F29" s="4"/>
-      <c r="G29" s="2"/>
+      <c r="G29" s="2">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C30" s="5"/>
@@ -876,8 +890,8 @@
         <v>3</v>
       </c>
       <c r="G39" s="1">
-        <f>SUM(G4:G27)</f>
-        <v>26</v>
+        <f>SUM(G4:G29)</f>
+        <v>30.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Runner & Merchant completly working
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -114,6 +114,9 @@
   </si>
   <si>
     <t>Runner update(80%) &amp; general data update</t>
+  </si>
+  <si>
+    <t>Runner &amp; Merchant completly working</t>
   </si>
 </sst>
 </file>
@@ -510,8 +513,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -830,11 +833,15 @@
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" s="5"/>
+      <c r="C30" s="5" t="s">
+        <v>30</v>
+      </c>
       <c r="D30" s="4"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4"/>
-      <c r="G30" s="2"/>
+      <c r="G30" s="2">
+        <v>4</v>
+      </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C31" s="5"/>
@@ -890,8 +897,8 @@
         <v>3</v>
       </c>
       <c r="G39" s="1">
-        <f>SUM(G4:G29)</f>
-        <v>30.7</v>
+        <f>SUM(G4:G30)</f>
+        <v>34.700000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
random data & output update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -117,6 +117,12 @@
   </si>
   <si>
     <t>Runner &amp; Merchant completly working</t>
+  </si>
+  <si>
+    <t>#include &amp; constructors update &amp; source added</t>
+  </si>
+  <si>
+    <t>random data &amp; output update</t>
   </si>
 </sst>
 </file>
@@ -513,8 +519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C31" sqref="C31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="G33" sqref="G33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -844,18 +850,26 @@
       </c>
     </row>
     <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" s="5"/>
+      <c r="C31" s="5" t="s">
+        <v>31</v>
+      </c>
       <c r="D31" s="4"/>
       <c r="E31" s="4"/>
       <c r="F31" s="4"/>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2">
+        <v>3.5</v>
+      </c>
     </row>
     <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" s="5"/>
+      <c r="C32" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="D32" s="4"/>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
-      <c r="G32" s="2"/>
+      <c r="G32" s="2">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C33" s="5"/>
@@ -897,8 +911,8 @@
         <v>3</v>
       </c>
       <c r="G39" s="1">
-        <f>SUM(G4:G30)</f>
-        <v>34.700000000000003</v>
+        <f>SUM(G4:G32)</f>
+        <v>40.700000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
game source update & potions added
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>random data &amp; output update</t>
+  </si>
+  <si>
+    <t>game source update &amp; potions added</t>
   </si>
 </sst>
 </file>
@@ -519,8 +522,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -872,11 +875,15 @@
       </c>
     </row>
     <row r="33" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C33" s="5"/>
+      <c r="C33" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="D33" s="4"/>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="2"/>
+      <c r="G33" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C34" s="5"/>
@@ -911,8 +918,8 @@
         <v>3</v>
       </c>
       <c r="G39" s="1">
-        <f>SUM(G4:G32)</f>
-        <v>40.700000000000003</v>
+        <f>SUM(G4:G33)</f>
+        <v>42.7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
potions working & object classes update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>game source update &amp; potions added</t>
+  </si>
+  <si>
+    <t>potions working &amp; object classes update</t>
   </si>
 </sst>
 </file>
@@ -522,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,11 +889,15 @@
       </c>
     </row>
     <row r="34" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C34" s="5"/>
+      <c r="C34" s="5" t="s">
+        <v>34</v>
+      </c>
       <c r="D34" s="4"/>
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
-      <c r="G34" s="2"/>
+      <c r="G34" s="2">
+        <v>1.8</v>
+      </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C35" s="5"/>
@@ -918,8 +925,8 @@
         <v>3</v>
       </c>
       <c r="G39" s="1">
-        <f>SUM(G4:G33)</f>
-        <v>42.7</v>
+        <f>SUM(G4:G34)</f>
+        <v>44.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
world reorganization & data workflow update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -129,6 +129,9 @@
   </si>
   <si>
     <t>potions working &amp; object classes update</t>
+  </si>
+  <si>
+    <t>world reorganization &amp; data workflow update</t>
   </si>
 </sst>
 </file>
@@ -525,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -900,11 +903,15 @@
       </c>
     </row>
     <row r="35" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C35" s="5"/>
+      <c r="C35" s="5" t="s">
+        <v>35</v>
+      </c>
       <c r="D35" s="4"/>
       <c r="E35" s="4"/>
       <c r="F35" s="4"/>
-      <c r="G35" s="2"/>
+      <c r="G35" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="36" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C36" s="5"/>
@@ -925,8 +932,8 @@
         <v>3</v>
       </c>
       <c r="G39" s="1">
-        <f>SUM(G4:G34)</f>
-        <v>44.5</v>
+        <f>SUM(G4:G35)</f>
+        <v>47.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
extern source update & bugs fixed
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -132,13 +132,16 @@
   </si>
   <si>
     <t>world reorganization &amp; data workflow update</t>
+  </si>
+  <si>
+    <t>external source update &amp; bugs fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -170,6 +173,14 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -235,13 +246,14 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="3"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="20% - Énfasis5" xfId="4" builtinId="46"/>
@@ -526,9 +538,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
       <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
@@ -880,7 +892,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="33" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="5" t="s">
         <v>33</v>
       </c>
@@ -891,7 +903,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C34" s="5" t="s">
         <v>34</v>
       </c>
@@ -902,7 +914,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="35" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C35" s="5" t="s">
         <v>35</v>
       </c>
@@ -913,27 +925,102 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C36" s="5"/>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="5" t="s">
+        <v>36</v>
+      </c>
       <c r="D36" s="4"/>
       <c r="E36" s="4"/>
       <c r="F36" s="4"/>
-      <c r="G36" s="2"/>
-    </row>
-    <row r="37" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C37" s="5"/>
       <c r="D37" s="4"/>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="2"/>
     </row>
-    <row r="39" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="F39" s="1" t="s">
+    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C38" s="5"/>
+      <c r="D38" s="4"/>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="2"/>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="5"/>
+      <c r="D39" s="4"/>
+      <c r="E39" s="4"/>
+      <c r="F39" s="4"/>
+      <c r="G39" s="2"/>
+    </row>
+    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C40" s="5"/>
+      <c r="D40" s="4"/>
+      <c r="E40" s="4"/>
+      <c r="F40" s="4"/>
+      <c r="G40" s="2"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="5"/>
+      <c r="D41" s="4"/>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="2"/>
+      <c r="I41" s="6"/>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="5"/>
+      <c r="D42" s="4"/>
+      <c r="E42" s="4"/>
+      <c r="F42" s="4"/>
+      <c r="G42" s="2"/>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="5"/>
+      <c r="D43" s="4"/>
+      <c r="E43" s="4"/>
+      <c r="F43" s="4"/>
+      <c r="G43" s="2"/>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="5"/>
+      <c r="D44" s="4"/>
+      <c r="E44" s="4"/>
+      <c r="F44" s="4"/>
+      <c r="G44" s="2"/>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="5"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+      <c r="G45" s="2"/>
+    </row>
+    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C46" s="5"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
+      <c r="F46" s="4"/>
+      <c r="G46" s="2"/>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C47" s="5"/>
+      <c r="D47" s="4"/>
+      <c r="E47" s="4"/>
+      <c r="F47" s="4"/>
+      <c r="G47" s="2"/>
+    </row>
+    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+      <c r="F49" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="G39" s="1">
-        <f>SUM(G4:G35)</f>
-        <v>47.5</v>
+      <c r="G49" s="1">
+        <f>SUM(G4:G36)</f>
+        <v>50.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fight system & game update update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>arena room update</t>
+  </si>
+  <si>
+    <t>fight system &amp; game update update</t>
   </si>
 </sst>
 </file>
@@ -544,7 +547,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C38" sqref="C38"/>
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -951,11 +954,15 @@
       </c>
     </row>
     <row r="38" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C38" s="5"/>
+      <c r="C38" s="5" t="s">
+        <v>38</v>
+      </c>
       <c r="D38" s="4"/>
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
-      <c r="G38" s="2"/>
+      <c r="G38" s="2">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C39" s="5"/>
@@ -1026,8 +1033,8 @@
         <v>3</v>
       </c>
       <c r="G49" s="1">
-        <f>SUM(G4:G37)</f>
-        <v>54.5</v>
+        <f>SUM(G4:G38)</f>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slim printf created & added
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>fight system &amp; game update update</t>
+  </si>
+  <si>
+    <t>slim printf created &amp; added</t>
   </si>
 </sst>
 </file>
@@ -547,7 +550,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C39" sqref="C39"/>
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -965,11 +968,15 @@
       </c>
     </row>
     <row r="39" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C39" s="5"/>
+      <c r="C39" s="5" t="s">
+        <v>39</v>
+      </c>
       <c r="D39" s="4"/>
       <c r="E39" s="4"/>
       <c r="F39" s="4"/>
-      <c r="G39" s="2"/>
+      <c r="G39" s="2">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="40" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C40" s="5"/>
@@ -1033,8 +1040,8 @@
         <v>3</v>
       </c>
       <c r="G49" s="1">
-        <f>SUM(G4:G38)</f>
-        <v>57</v>
+        <f>SUM(G4:G39)</f>
+        <v>61.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
RESET update & bugs fixed
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -1,22 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuari\Desktop\Arena_Game\ARENA\Arena_Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4507"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20730" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <calcPr calcId="125725"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -144,13 +139,19 @@
   </si>
   <si>
     <t>slim printf created &amp; added</t>
+  </si>
+  <si>
+    <t>arena win/lose conditions added</t>
+  </si>
+  <si>
+    <t>RESET update &amp; bugs fixed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,7 +328,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -362,7 +363,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -539,32 +540,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D40" sqref="D40"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="C42" sqref="C42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="5" max="5" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="C2" s="4" t="s">
         <v>2</v>
       </c>
@@ -575,14 +576,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="C4" s="4" t="s">
         <v>1</v>
       </c>
@@ -593,7 +594,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
@@ -604,7 +605,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="C6" s="5" t="s">
         <v>5</v>
       </c>
@@ -615,7 +616,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="C7" s="5" t="s">
         <v>7</v>
       </c>
@@ -626,7 +627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="C8" s="5" t="s">
         <v>8</v>
       </c>
@@ -637,7 +638,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="C9" s="5" t="s">
         <v>9</v>
       </c>
@@ -648,7 +649,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="C10" s="5" t="s">
         <v>10</v>
       </c>
@@ -659,7 +660,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="C11" s="5" t="s">
         <v>11</v>
       </c>
@@ -670,7 +671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="C12" s="5" t="s">
         <v>12</v>
       </c>
@@ -681,7 +682,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="C13" s="5" t="s">
         <v>13</v>
       </c>
@@ -692,7 +693,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="C14" s="5" t="s">
         <v>14</v>
       </c>
@@ -703,7 +704,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7">
       <c r="C15" s="5" t="s">
         <v>15</v>
       </c>
@@ -714,7 +715,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7">
       <c r="C16" s="5" t="s">
         <v>16</v>
       </c>
@@ -725,7 +726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7">
       <c r="C17" s="5" t="s">
         <v>17</v>
       </c>
@@ -736,7 +737,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7">
       <c r="C18" s="5" t="s">
         <v>18</v>
       </c>
@@ -747,7 +748,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7">
       <c r="C19" s="5" t="s">
         <v>19</v>
       </c>
@@ -758,7 +759,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="20" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:7">
       <c r="C20" s="5" t="s">
         <v>20</v>
       </c>
@@ -769,7 +770,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="21" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:7">
       <c r="C21" s="5" t="s">
         <v>21</v>
       </c>
@@ -780,7 +781,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="22" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:7">
       <c r="C22" s="5" t="s">
         <v>22</v>
       </c>
@@ -791,7 +792,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="3:7">
       <c r="C23" s="5" t="s">
         <v>23</v>
       </c>
@@ -802,7 +803,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:7">
       <c r="C24" s="5" t="s">
         <v>24</v>
       </c>
@@ -813,7 +814,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="25" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:7">
       <c r="C25" s="5" t="s">
         <v>25</v>
       </c>
@@ -824,7 +825,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:7">
       <c r="C26" s="5" t="s">
         <v>26</v>
       </c>
@@ -835,7 +836,7 @@
         <v>1.2</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:7">
       <c r="C27" s="5" t="s">
         <v>27</v>
       </c>
@@ -846,7 +847,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:7">
       <c r="C28" s="5" t="s">
         <v>28</v>
       </c>
@@ -857,7 +858,7 @@
         <v>2.2000000000000002</v>
       </c>
     </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:7">
       <c r="C29" s="5" t="s">
         <v>29</v>
       </c>
@@ -868,7 +869,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:7">
       <c r="C30" s="5" t="s">
         <v>30</v>
       </c>
@@ -879,7 +880,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:7">
       <c r="C31" s="5" t="s">
         <v>31</v>
       </c>
@@ -890,7 +891,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:7">
       <c r="C32" s="5" t="s">
         <v>32</v>
       </c>
@@ -901,7 +902,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:9">
       <c r="C33" s="5" t="s">
         <v>33</v>
       </c>
@@ -912,7 +913,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:9">
       <c r="C34" s="5" t="s">
         <v>34</v>
       </c>
@@ -923,7 +924,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:9">
       <c r="C35" s="5" t="s">
         <v>35</v>
       </c>
@@ -934,7 +935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:9">
       <c r="C36" s="5" t="s">
         <v>36</v>
       </c>
@@ -945,7 +946,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:9">
       <c r="C37" s="5" t="s">
         <v>37</v>
       </c>
@@ -956,7 +957,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:9">
       <c r="C38" s="5" t="s">
         <v>38</v>
       </c>
@@ -967,7 +968,7 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:9">
       <c r="C39" s="5" t="s">
         <v>39</v>
       </c>
@@ -978,70 +979,78 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="40" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C40" s="5"/>
+    <row r="40" spans="3:9">
+      <c r="C40" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="D40" s="4"/>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
-      <c r="G40" s="2"/>
-    </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
-      <c r="C41" s="5"/>
+      <c r="G40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="3:9">
+      <c r="C41" s="5" t="s">
+        <v>41</v>
+      </c>
       <c r="D41" s="4"/>
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
-      <c r="G41" s="2"/>
+      <c r="G41" s="2">
+        <v>2.5</v>
+      </c>
       <c r="I41" s="6"/>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:9">
       <c r="C42" s="5"/>
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
       <c r="G42" s="2"/>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:9">
       <c r="C43" s="5"/>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="2"/>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:9">
       <c r="C44" s="5"/>
       <c r="D44" s="4"/>
       <c r="E44" s="4"/>
       <c r="F44" s="4"/>
       <c r="G44" s="2"/>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:9">
       <c r="C45" s="5"/>
       <c r="D45" s="4"/>
       <c r="E45" s="4"/>
       <c r="F45" s="4"/>
       <c r="G45" s="2"/>
     </row>
-    <row r="46" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:9">
       <c r="C46" s="5"/>
       <c r="D46" s="4"/>
       <c r="E46" s="4"/>
       <c r="F46" s="4"/>
       <c r="G46" s="2"/>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:9">
       <c r="C47" s="5"/>
       <c r="D47" s="4"/>
       <c r="E47" s="4"/>
       <c r="F47" s="4"/>
       <c r="G47" s="2"/>
     </row>
-    <row r="49" spans="6:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="6:7">
       <c r="F49" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G49" s="1">
-        <f>SUM(G4:G39)</f>
-        <v>61.5</v>
+        <f>SUM(G4:G41)</f>
+        <v>66</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
arena & creatures update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -148,6 +148,9 @@
   </si>
   <si>
     <t>visual game update</t>
+  </si>
+  <si>
+    <t>arena &amp; creatures update</t>
   </si>
 </sst>
 </file>
@@ -543,7 +546,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -554,7 +557,7 @@
   <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1017,11 +1020,15 @@
       </c>
     </row>
     <row r="43" spans="3:9">
-      <c r="C43" s="5"/>
+      <c r="C43" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="2"/>
+      <c r="G43" s="2">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="44" spans="3:9">
       <c r="C44" s="5"/>
@@ -1056,8 +1063,8 @@
         <v>3</v>
       </c>
       <c r="G49" s="1">
-        <f>SUM(G4:G42)</f>
-        <v>68</v>
+        <f>SUM(G4:G43)</f>
+        <v>69.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
potions & runes workflow update(70%)
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t>potions updated</t>
+  </si>
+  <si>
+    <t>potions &amp; runes workflow update(70%)</t>
   </si>
 </sst>
 </file>
@@ -561,7 +564,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -571,8 +574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1101,11 +1104,15 @@
       </c>
     </row>
     <row r="49" spans="3:7">
-      <c r="C49" s="5"/>
+      <c r="C49" s="5" t="s">
+        <v>49</v>
+      </c>
       <c r="D49" s="4"/>
       <c r="E49" s="4"/>
       <c r="F49" s="4"/>
-      <c r="G49" s="2"/>
+      <c r="G49" s="2">
+        <v>2.2999999999999998</v>
+      </c>
     </row>
     <row r="50" spans="3:7">
       <c r="C50" s="5"/>
@@ -1182,8 +1189,8 @@
         <v>3</v>
       </c>
       <c r="G61" s="1">
-        <f>SUM(G4:G48)</f>
-        <v>77.5</v>
+        <f>SUM(G4:G49)</f>
+        <v>79.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
const buffs completed & some bugs fixed
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -169,6 +169,9 @@
   </si>
   <si>
     <t>potions &amp; runes workflow update(70%)</t>
+  </si>
+  <si>
+    <t>const buffs completed &amp; some bugs fixed</t>
   </si>
 </sst>
 </file>
@@ -564,7 +567,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -575,7 +578,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+      <selection activeCell="C50" sqref="C50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1115,11 +1118,15 @@
       </c>
     </row>
     <row r="50" spans="3:7">
-      <c r="C50" s="5"/>
+      <c r="C50" s="5" t="s">
+        <v>50</v>
+      </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
       <c r="F50" s="4"/>
-      <c r="G50" s="2"/>
+      <c r="G50" s="2">
+        <v>3</v>
+      </c>
     </row>
     <row r="51" spans="3:7">
       <c r="C51" s="5"/>
@@ -1189,8 +1196,8 @@
         <v>3</v>
       </c>
       <c r="G61" s="1">
-        <f>SUM(G4:G49)</f>
-        <v>79.8</v>
+        <f>SUM(G4:G50)</f>
+        <v>82.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tamer & pets added & constructors update
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -172,6 +172,9 @@
   </si>
   <si>
     <t>const buffs completed &amp; some bugs fixed</t>
+  </si>
+  <si>
+    <t>tamer &amp; pets added &amp; constructors update</t>
   </si>
 </sst>
 </file>
@@ -567,7 +570,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -578,7 +581,7 @@
   <dimension ref="A1:I61"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1129,11 +1132,15 @@
       </c>
     </row>
     <row r="51" spans="3:7">
-      <c r="C51" s="5"/>
+      <c r="C51" s="5" t="s">
+        <v>51</v>
+      </c>
       <c r="D51" s="4"/>
       <c r="E51" s="4"/>
       <c r="F51" s="4"/>
-      <c r="G51" s="2"/>
+      <c r="G51" s="2">
+        <v>5.5</v>
+      </c>
     </row>
     <row r="52" spans="3:7">
       <c r="C52" s="5"/>
@@ -1196,8 +1203,8 @@
         <v>3</v>
       </c>
       <c r="G61" s="1">
-        <f>SUM(G4:G50)</f>
-        <v>82.8</v>
+        <f>SUM(G4:G51)</f>
+        <v>88.3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
now you can buy pets & look it
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -175,6 +175,9 @@
   </si>
   <si>
     <t>tamer &amp; pets added &amp; constructors update</t>
+  </si>
+  <si>
+    <t>now you can buy pets &amp; look it</t>
   </si>
 </sst>
 </file>
@@ -570,7 +573,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -580,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1143,11 +1146,15 @@
       </c>
     </row>
     <row r="52" spans="3:7">
-      <c r="C52" s="5"/>
+      <c r="C52" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="D52" s="4"/>
       <c r="E52" s="4"/>
       <c r="F52" s="4"/>
-      <c r="G52" s="2"/>
+      <c r="G52" s="2">
+        <v>2.5</v>
+      </c>
     </row>
     <row r="53" spans="3:7">
       <c r="C53" s="5"/>
@@ -1203,8 +1210,8 @@
         <v>3</v>
       </c>
       <c r="G61" s="1">
-        <f>SUM(G4:G51)</f>
-        <v>88.3</v>
+        <f>SUM(G4:G52)</f>
+        <v>90.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
pets working & bugs fixed
</commit_message>
<xml_diff>
--- a/Arena_Data/Commits table.xlsx
+++ b/Arena_Data/Commits table.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>ARENA COMMITS TABLE:</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>now you can buy pets &amp; look it</t>
+  </si>
+  <si>
+    <t>pets working &amp; bugs fixed</t>
   </si>
 </sst>
 </file>
@@ -573,7 +576,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -583,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:I61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="C54" sqref="C54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1157,11 +1160,15 @@
       </c>
     </row>
     <row r="53" spans="3:7">
-      <c r="C53" s="5"/>
+      <c r="C53" s="5" t="s">
+        <v>53</v>
+      </c>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
       <c r="F53" s="4"/>
-      <c r="G53" s="2"/>
+      <c r="G53" s="2">
+        <v>2</v>
+      </c>
     </row>
     <row r="54" spans="3:7">
       <c r="C54" s="5"/>
@@ -1210,8 +1217,8 @@
         <v>3</v>
       </c>
       <c r="G61" s="1">
-        <f>SUM(G4:G52)</f>
-        <v>90.8</v>
+        <f>SUM(G4:G53)</f>
+        <v>92.8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>